<commit_message>
[TimesheetCalculatorV2] Changes: * implemented holidays * fixed test errors * moved the parameters of employee and task_list  from instantiation to its actual calling method. * updated test accordingly
</commit_message>
<xml_diff>
--- a/python_source/Timesheet_Calculator_v2/test/business_logic/testdata/ss_generator_testdata_001.xlsx
+++ b/python_source/Timesheet_Calculator_v2/test/business_logic/testdata/ss_generator_testdata_001.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="46">
   <si>
     <t xml:space="preserve">PTCC TIMESHEET FOR WEEK (07-Jun-2021 to 21-Jun-2021)</t>
   </si>
@@ -131,7 +131,7 @@
     <t xml:space="preserve">FRI</t>
   </si>
   <si>
-    <t xml:space="preserve">12-Jun-2021</t>
+    <t xml:space="preserve">12-Jun-2021 (HOLIDAY)</t>
   </si>
   <si>
     <t xml:space="preserve">SAT</t>
@@ -299,11 +299,11 @@
   </sheetPr>
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="80.9"/>
@@ -416,14 +416,14 @@
   </sheetPr>
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E32" activeCellId="0" sqref="E32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="44.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="31.21"/>
@@ -577,14 +577,17 @@
       <c r="B12" s="0" t="s">
         <v>34</v>
       </c>
+      <c r="C12" s="0" t="s">
+        <v>26</v>
+      </c>
       <c r="D12" s="0" t="n">
-        <v>0</v>
+        <v>480</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F12" s="0" t="n">
-        <v>0</v>
+        <v>480</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
[TimesheetCalculatorV2] Changes: * removed initialization of model in main. moved it when user clicks the generate button * added rerun implementation. and implemented stop and closing during execution. * implemented progress message signal and slot and updated in the UI. * added display message in the UI implementation. * added ui implementation for rerun, closing and stopping. * added the implementation for adjusting cell width and height. for each cell using approximation of openpyxl. * removed the default sheet during the final creation of the output.
</commit_message>
<xml_diff>
--- a/python_source/Timesheet_Calculator_v2/test/business_logic/testdata/ss_generator_testdata_001.xlsx
+++ b/python_source/Timesheet_Calculator_v2/test/business_logic/testdata/ss_generator_testdata_001.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
     <t xml:space="preserve">PTCC TIMESHEET FOR WEEK (07-Jun-2021 to 21-Jun-2021)</t>
   </si>
   <si>
-    <t xml:space="preserve">14-June-2021</t>
+    <t xml:space="preserve">15-June-2021</t>
   </si>
   <si>
     <t xml:space="preserve">NAME</t>
@@ -299,11 +299,11 @@
   </sheetPr>
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="80.9"/>
@@ -416,11 +416,11 @@
   </sheetPr>
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="44.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.62"/>

</xml_diff>

<commit_message>
[TimesheetCalculatorV2] Changes: * implemented applying bold and borders in cells. * updated testdata
</commit_message>
<xml_diff>
--- a/python_source/Timesheet_Calculator_v2/test/business_logic/testdata/ss_generator_testdata_001.xlsx
+++ b/python_source/Timesheet_Calculator_v2/test/business_logic/testdata/ss_generator_testdata_001.xlsx
@@ -26,7 +26,7 @@
     <t xml:space="preserve">PTCC TIMESHEET FOR WEEK (07-Jun-2021 to 21-Jun-2021)</t>
   </si>
   <si>
-    <t xml:space="preserve">15-June-2021</t>
+    <t xml:space="preserve">16-June-2021</t>
   </si>
   <si>
     <t xml:space="preserve">NAME</t>
@@ -300,10 +300,10 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="80.9"/>
@@ -420,7 +420,7 @@
       <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="44.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.62"/>

</xml_diff>